<commit_message>
tests: extending excel importer to svein harald
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-addition-svein-harald.xlsx
+++ b/docs/artifacts/rules/information-addition-svein-harald.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4FB99-C3AA-44D7-8ECD-7CFE1B4C9BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B227FDB-D479-4661-97F4-1EB53086169D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Classes" sheetId="3" r:id="rId3"/>
     <sheet name="LastProperties" sheetId="4" r:id="rId4"/>
     <sheet name="LastClasses" sheetId="5" r:id="rId5"/>
+    <sheet name="LastMetadata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
   <si>
     <t>role</t>
   </si>
@@ -381,12 +382,21 @@
   </si>
   <si>
     <t>Inf</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>Jon,Emma,David,Alice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -471,6 +481,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2949,4 +2960,126 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6EF7B3-3653-43A9-A64A-DCF274C66021}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7">
+        <v>45431.300828611107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="7">
+        <v>45431.300828611107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>